<commit_message>
2 new data and reruns
</commit_message>
<xml_diff>
--- a/DorozeaStreamStats.xlsx
+++ b/DorozeaStreamStats.xlsx
@@ -1441,6 +1441,20 @@
         <v>108.0</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" s="1">
+        <v>82.0</v>
+      </c>
+      <c r="B84" s="1">
+        <v>247.0</v>
+      </c>
+      <c r="C84" s="1">
+        <v>333.0</v>
+      </c>
+      <c r="D84" s="1">
+        <v>105.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
8-5 data + rerun
</commit_message>
<xml_diff>
--- a/DorozeaStreamStats.xlsx
+++ b/DorozeaStreamStats.xlsx
@@ -1455,6 +1455,20 @@
         <v>105.0</v>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" s="1">
+        <v>83.0</v>
+      </c>
+      <c r="B85" s="1">
+        <v>179.0</v>
+      </c>
+      <c r="C85" s="1">
+        <v>214.0</v>
+      </c>
+      <c r="D85" s="1">
+        <v>67.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
8-23 and re runs
</commit_message>
<xml_diff>
--- a/DorozeaStreamStats.xlsx
+++ b/DorozeaStreamStats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>stream</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>jc, ow2, rdr2, marbels</t>
+  </si>
+  <si>
+    <t>jc, lol, cs, rdr2, marbels</t>
   </si>
 </sst>
 </file>
@@ -2032,6 +2035,23 @@
         <v>49</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" s="1">
+        <v>92.0</v>
+      </c>
+      <c r="B94" s="1">
+        <v>214.0</v>
+      </c>
+      <c r="C94" s="1">
+        <v>262.0</v>
+      </c>
+      <c r="D94" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
big reruns and new stuff
</commit_message>
<xml_diff>
--- a/DorozeaStreamStats.xlsx
+++ b/DorozeaStreamStats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="140">
   <si>
     <t>stream</t>
   </si>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t>jc, lol, batman3</t>
+  </si>
+  <si>
+    <t>jc, marvel, lol, marbels</t>
   </si>
 </sst>
 </file>
@@ -4457,6 +4460,57 @@
         <v>37</v>
       </c>
     </row>
+    <row r="222">
+      <c r="A222" s="1">
+        <v>220.0</v>
+      </c>
+      <c r="B222" s="1">
+        <v>644.0</v>
+      </c>
+      <c r="C222" s="1">
+        <v>746.0</v>
+      </c>
+      <c r="D222" s="1">
+        <v>560.0</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1">
+        <v>221.0</v>
+      </c>
+      <c r="B223" s="1">
+        <v>622.0</v>
+      </c>
+      <c r="C223" s="1">
+        <v>925.0</v>
+      </c>
+      <c r="D223" s="1">
+        <v>270.0</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1">
+        <v>222.0</v>
+      </c>
+      <c r="B224" s="1">
+        <v>916.0</v>
+      </c>
+      <c r="C224" s="1">
+        <v>1123.0</v>
+      </c>
+      <c r="D224" s="1">
+        <v>427.0</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
new garp and rerun 12hours stream
</commit_message>
<xml_diff>
--- a/DorozeaStreamStats.xlsx
+++ b/DorozeaStreamStats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="174">
   <si>
     <t>stream</t>
   </si>
@@ -530,6 +530,9 @@
   </si>
   <si>
     <t>jc, garlicshow, cs, marvels, cp</t>
+  </si>
+  <si>
+    <t>jc, lol, garlicshow, sus, repo, roblox, cs, marbels</t>
   </si>
 </sst>
 </file>
@@ -5528,6 +5531,23 @@
         <v>172</v>
       </c>
     </row>
+    <row r="279">
+      <c r="A279" s="1">
+        <v>277.0</v>
+      </c>
+      <c r="B279" s="1">
+        <v>991.0</v>
+      </c>
+      <c r="C279" s="1">
+        <v>1726.0</v>
+      </c>
+      <c r="D279" s="1">
+        <v>388.0</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
6-20 and  6- 21
</commit_message>
<xml_diff>
--- a/DorozeaStreamStats.xlsx
+++ b/DorozeaStreamStats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="215">
   <si>
     <t>stream</t>
   </si>
@@ -6827,6 +6827,40 @@
         <v>76</v>
       </c>
     </row>
+    <row r="348">
+      <c r="A348" s="1">
+        <v>346.0</v>
+      </c>
+      <c r="B348" s="1">
+        <v>1019.0</v>
+      </c>
+      <c r="C348" s="1">
+        <v>1338.0</v>
+      </c>
+      <c r="D348" s="1">
+        <v>143.0</v>
+      </c>
+      <c r="E348" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="1">
+        <v>347.0</v>
+      </c>
+      <c r="B349" s="1">
+        <v>1239.0</v>
+      </c>
+      <c r="C349" s="1">
+        <v>1618.0</v>
+      </c>
+      <c r="D349" s="1">
+        <v>538.0</v>
+      </c>
+      <c r="E349" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
11-4 is good but not from vod
</commit_message>
<xml_diff>
--- a/DorozeaStreamStats.xlsx
+++ b/DorozeaStreamStats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="277">
   <si>
     <t>stream</t>
   </si>
@@ -839,6 +839,9 @@
   </si>
   <si>
     <t>jc, cs, ow2, rvthereyet</t>
+  </si>
+  <si>
+    <t>jc, cs, devour</t>
   </si>
 </sst>
 </file>
@@ -8938,7 +8941,7 @@
         <v>459.0</v>
       </c>
       <c r="B461" s="1">
-        <v>569.0</v>
+        <v>609.0</v>
       </c>
       <c r="C461" s="1">
         <v>1118.0</v>
@@ -8955,7 +8958,7 @@
         <v>460.0</v>
       </c>
       <c r="B462" s="1">
-        <v>972.0</v>
+        <v>978.0</v>
       </c>
       <c r="C462" s="1">
         <v>1129.0</v>
@@ -8972,7 +8975,7 @@
         <v>461.0</v>
       </c>
       <c r="B463" s="1">
-        <v>855.0</v>
+        <v>857.0</v>
       </c>
       <c r="C463" s="1">
         <v>926.0</v>
@@ -8989,7 +8992,7 @@
         <v>462.0</v>
       </c>
       <c r="B464" s="1">
-        <v>892.0</v>
+        <v>898.0</v>
       </c>
       <c r="C464" s="1">
         <v>1009.0</v>
@@ -8999,6 +9002,58 @@
       </c>
       <c r="E464" s="1" t="s">
         <v>275</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="1">
+        <v>563.0</v>
+      </c>
+      <c r="B465" s="1">
+        <v>791.0</v>
+      </c>
+      <c r="C465" s="1">
+        <v>1019.0</v>
+      </c>
+      <c r="D465" s="1">
+        <v>138.0</v>
+      </c>
+      <c r="E465" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F465" s="1"/>
+    </row>
+    <row r="466">
+      <c r="A466" s="1">
+        <v>564.0</v>
+      </c>
+      <c r="B466" s="1">
+        <v>1053.0</v>
+      </c>
+      <c r="C466" s="1">
+        <v>1709.0</v>
+      </c>
+      <c r="D466" s="1">
+        <v>164.0</v>
+      </c>
+      <c r="E466" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="1">
+        <v>565.0</v>
+      </c>
+      <c r="B467" s="1">
+        <v>1025.0</v>
+      </c>
+      <c r="C467" s="1">
+        <v>1322.0</v>
+      </c>
+      <c r="D467" s="1">
+        <v>74.0</v>
+      </c>
+      <c r="E467" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2-3 and delete some old datajsons
</commit_message>
<xml_diff>
--- a/DorozeaStreamStats.xlsx
+++ b/DorozeaStreamStats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="289">
   <si>
     <t>stream</t>
   </si>
@@ -875,6 +875,9 @@
   </si>
   <si>
     <t>jc, cs, fornite, devour</t>
+  </si>
+  <si>
+    <t>jc, fortnite, arc, marbels</t>
   </si>
 </sst>
 </file>
@@ -9430,6 +9433,41 @@
         <v>10</v>
       </c>
     </row>
+    <row r="488">
+      <c r="A488" s="1">
+        <v>486.0</v>
+      </c>
+      <c r="B488" s="1">
+        <v>1006.0</v>
+      </c>
+      <c r="C488" s="1">
+        <v>1494.0</v>
+      </c>
+      <c r="D488" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="E488" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F488" s="1"/>
+    </row>
+    <row r="489">
+      <c r="A489" s="1">
+        <v>487.0</v>
+      </c>
+      <c r="B489" s="1">
+        <v>1160.0</v>
+      </c>
+      <c r="C489" s="1">
+        <v>1526.0</v>
+      </c>
+      <c r="D489" s="1">
+        <v>198.0</v>
+      </c>
+      <c r="E489" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
3 streams in jan 9
</commit_message>
<xml_diff>
--- a/DorozeaStreamStats.xlsx
+++ b/DorozeaStreamStats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="299">
   <si>
     <t>stream</t>
   </si>
@@ -9945,6 +9945,74 @@
         <v>130</v>
       </c>
     </row>
+    <row r="516">
+      <c r="A516" s="1">
+        <v>514.0</v>
+      </c>
+      <c r="B516" s="1">
+        <v>1436.0</v>
+      </c>
+      <c r="C516" s="1">
+        <v>1679.0</v>
+      </c>
+      <c r="D516" s="1">
+        <v>312.0</v>
+      </c>
+      <c r="E516" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" s="1">
+        <v>515.0</v>
+      </c>
+      <c r="B517" s="1">
+        <v>633.0</v>
+      </c>
+      <c r="C517" s="1">
+        <v>633.0</v>
+      </c>
+      <c r="D517" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="E517" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" s="1">
+        <v>516.0</v>
+      </c>
+      <c r="B518" s="1">
+        <v>1849.0</v>
+      </c>
+      <c r="C518" s="1">
+        <v>2190.0</v>
+      </c>
+      <c r="D518" s="1">
+        <v>140.0</v>
+      </c>
+      <c r="E518" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="1">
+        <v>517.0</v>
+      </c>
+      <c r="B519" s="1">
+        <v>1120.0</v>
+      </c>
+      <c r="C519" s="1">
+        <v>1529.0</v>
+      </c>
+      <c r="D519" s="1">
+        <v>-2.0</v>
+      </c>
+      <c r="E519" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update stream stats and add new data files
</commit_message>
<xml_diff>
--- a/DorozeaStreamStats.xlsx
+++ b/DorozeaStreamStats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="305">
   <si>
     <t>stream</t>
   </si>
@@ -920,6 +920,12 @@
   </si>
   <si>
     <t>jc, ds, marbels</t>
+  </si>
+  <si>
+    <t>jc, ds</t>
+  </si>
+  <si>
+    <t>jc, cs, ds</t>
   </si>
 </sst>
 </file>
@@ -10280,6 +10286,57 @@
         <v>302</v>
       </c>
     </row>
+    <row r="535">
+      <c r="A535" s="1">
+        <v>533.0</v>
+      </c>
+      <c r="B535" s="1">
+        <v>1189.0</v>
+      </c>
+      <c r="C535" s="1">
+        <v>1484.0</v>
+      </c>
+      <c r="D535" s="1">
+        <v>165.0</v>
+      </c>
+      <c r="E535" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="1">
+        <v>534.0</v>
+      </c>
+      <c r="B536" s="1">
+        <v>1213.0</v>
+      </c>
+      <c r="C536" s="1">
+        <v>1361.0</v>
+      </c>
+      <c r="D536" s="1">
+        <v>150.0</v>
+      </c>
+      <c r="E536" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="1">
+        <v>535.0</v>
+      </c>
+      <c r="B537" s="1">
+        <v>1249.0</v>
+      </c>
+      <c r="C537" s="1">
+        <v>1433.0</v>
+      </c>
+      <c r="D537" s="1">
+        <v>142.0</v>
+      </c>
+      <c r="E537" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
2 new stream and re runs
</commit_message>
<xml_diff>
--- a/DorozeaStreamStats.xlsx
+++ b/DorozeaStreamStats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="307">
   <si>
     <t>stream</t>
   </si>
@@ -10479,6 +10479,40 @@
         <v>15</v>
       </c>
     </row>
+    <row r="546">
+      <c r="A546" s="1">
+        <v>544.0</v>
+      </c>
+      <c r="B546" s="1">
+        <v>1110.0</v>
+      </c>
+      <c r="C546" s="1">
+        <v>1351.0</v>
+      </c>
+      <c r="D546" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="E546" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="1">
+        <v>545.0</v>
+      </c>
+      <c r="B547" s="1">
+        <v>625.0</v>
+      </c>
+      <c r="C547" s="1">
+        <v>781.0</v>
+      </c>
+      <c r="D547" s="1">
+        <v>33.0</v>
+      </c>
+      <c r="E547" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
addig 1more hour to the fixing chat logs
</commit_message>
<xml_diff>
--- a/DorozeaStreamStats.xlsx
+++ b/DorozeaStreamStats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="307">
   <si>
     <t>stream</t>
   </si>
@@ -10615,6 +10615,23 @@
         <v>15</v>
       </c>
     </row>
+    <row r="554">
+      <c r="A554" s="1">
+        <v>552.0</v>
+      </c>
+      <c r="B554" s="1">
+        <v>1211.0</v>
+      </c>
+      <c r="C554" s="1">
+        <v>1374.0</v>
+      </c>
+      <c r="D554" s="1">
+        <v>129.0</v>
+      </c>
+      <c r="E554" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>